<commit_message>
updated species list on clearing sheets
</commit_message>
<xml_diff>
--- a/Data Sheets/New England Kelp Clearing Data Sheet v1.5.1.xlsx
+++ b/Data Sheets/New England Kelp Clearing Data Sheet v1.5.1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="0" windowWidth="25440" windowHeight="14620" activeTab="2"/>
+    <workbookView xWindow="300" yWindow="0" windowWidth="30700" windowHeight="25120" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="27" r:id="rId1"/>
@@ -4366,6 +4366,47 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4402,46 +4443,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4461,7 +4462,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -7581,7 +7581,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="236">
+      <c r="A2" s="199">
         <v>42204</v>
       </c>
       <c r="B2" t="s">
@@ -7622,20 +7622,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="29" customFormat="1" ht="16" customHeight="1">
-      <c r="B1" s="213" t="s">
+      <c r="B1" s="209" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="213"/>
-      <c r="D1" s="213" t="s">
+      <c r="C1" s="209"/>
+      <c r="D1" s="209" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="213"/>
-      <c r="F1" s="213"/>
-      <c r="G1" s="214"/>
-      <c r="H1" s="221" t="s">
+      <c r="E1" s="209"/>
+      <c r="F1" s="209"/>
+      <c r="G1" s="210"/>
+      <c r="H1" s="217" t="s">
         <v>245</v>
       </c>
-      <c r="I1" s="214"/>
+      <c r="I1" s="210"/>
       <c r="J1" s="138"/>
       <c r="K1" s="138"/>
       <c r="L1" s="138"/>
@@ -7644,14 +7644,14 @@
       <c r="O1" s="138"/>
     </row>
     <row r="2" spans="1:15" s="29" customFormat="1" ht="16" customHeight="1">
-      <c r="B2" s="213"/>
-      <c r="C2" s="213"/>
-      <c r="D2" s="213"/>
-      <c r="E2" s="213"/>
-      <c r="F2" s="213"/>
-      <c r="G2" s="214"/>
-      <c r="H2" s="214"/>
-      <c r="I2" s="214"/>
+      <c r="B2" s="209"/>
+      <c r="C2" s="209"/>
+      <c r="D2" s="209"/>
+      <c r="E2" s="209"/>
+      <c r="F2" s="209"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
       <c r="J2" s="138"/>
       <c r="K2" s="138"/>
       <c r="L2" s="138"/>
@@ -7692,22 +7692,22 @@
     <row r="5" spans="1:15" s="27" customFormat="1" ht="34" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="135"/>
       <c r="B5" s="136"/>
-      <c r="C5" s="215" t="s">
+      <c r="C5" s="211" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="216"/>
-      <c r="E5" s="217" t="s">
+      <c r="D5" s="212"/>
+      <c r="E5" s="213" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="218"/>
-      <c r="G5" s="219" t="s">
+      <c r="F5" s="214"/>
+      <c r="G5" s="215" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="220"/>
-      <c r="I5" s="217" t="s">
+      <c r="H5" s="216"/>
+      <c r="I5" s="213" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="218"/>
+      <c r="J5" s="214"/>
       <c r="K5"/>
       <c r="L5"/>
       <c r="M5"/>
@@ -7718,14 +7718,14 @@
       <c r="B6" s="139" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="211"/>
-      <c r="D6" s="226"/>
-      <c r="E6" s="211"/>
-      <c r="F6" s="212"/>
-      <c r="G6" s="211"/>
-      <c r="H6" s="212"/>
-      <c r="I6" s="211"/>
-      <c r="J6" s="212"/>
+      <c r="C6" s="206"/>
+      <c r="D6" s="207"/>
+      <c r="E6" s="206"/>
+      <c r="F6" s="208"/>
+      <c r="G6" s="206"/>
+      <c r="H6" s="208"/>
+      <c r="I6" s="206"/>
+      <c r="J6" s="208"/>
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
@@ -7736,14 +7736,14 @@
       <c r="B7" s="140" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="224"/>
-      <c r="D7" s="225"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="225"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="225"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="225"/>
+      <c r="C7" s="202"/>
+      <c r="D7" s="203"/>
+      <c r="E7" s="202"/>
+      <c r="F7" s="203"/>
+      <c r="G7" s="202"/>
+      <c r="H7" s="203"/>
+      <c r="I7" s="202"/>
+      <c r="J7" s="203"/>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
@@ -7754,14 +7754,14 @@
       <c r="B8" s="141" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="222"/>
-      <c r="D8" s="223"/>
-      <c r="E8" s="222"/>
-      <c r="F8" s="223"/>
-      <c r="G8" s="222"/>
-      <c r="H8" s="223"/>
-      <c r="I8" s="222"/>
-      <c r="J8" s="223"/>
+      <c r="C8" s="200"/>
+      <c r="D8" s="201"/>
+      <c r="E8" s="200"/>
+      <c r="F8" s="201"/>
+      <c r="G8" s="200"/>
+      <c r="H8" s="201"/>
+      <c r="I8" s="200"/>
+      <c r="J8" s="201"/>
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
@@ -7772,14 +7772,14 @@
       <c r="B9" s="142" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="222"/>
-      <c r="D9" s="223"/>
-      <c r="E9" s="222"/>
-      <c r="F9" s="223"/>
-      <c r="G9" s="222"/>
-      <c r="H9" s="223"/>
-      <c r="I9" s="222"/>
-      <c r="J9" s="223"/>
+      <c r="C9" s="200"/>
+      <c r="D9" s="201"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="201"/>
+      <c r="G9" s="200"/>
+      <c r="H9" s="201"/>
+      <c r="I9" s="200"/>
+      <c r="J9" s="201"/>
       <c r="K9"/>
       <c r="L9"/>
       <c r="M9"/>
@@ -7790,14 +7790,14 @@
       <c r="B10" s="142" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="222"/>
-      <c r="D10" s="223"/>
-      <c r="E10" s="222"/>
-      <c r="F10" s="223"/>
-      <c r="G10" s="222"/>
-      <c r="H10" s="223"/>
-      <c r="I10" s="222"/>
-      <c r="J10" s="223"/>
+      <c r="C10" s="200"/>
+      <c r="D10" s="201"/>
+      <c r="E10" s="200"/>
+      <c r="F10" s="201"/>
+      <c r="G10" s="200"/>
+      <c r="H10" s="201"/>
+      <c r="I10" s="200"/>
+      <c r="J10" s="201"/>
       <c r="K10"/>
       <c r="L10"/>
       <c r="M10"/>
@@ -7808,14 +7808,14 @@
       <c r="B11" s="142" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="227"/>
-      <c r="D11" s="228"/>
-      <c r="E11" s="227"/>
-      <c r="F11" s="228"/>
-      <c r="G11" s="227"/>
-      <c r="H11" s="228"/>
-      <c r="I11" s="227"/>
-      <c r="J11" s="228"/>
+      <c r="C11" s="204"/>
+      <c r="D11" s="205"/>
+      <c r="E11" s="204"/>
+      <c r="F11" s="205"/>
+      <c r="G11" s="204"/>
+      <c r="H11" s="205"/>
+      <c r="I11" s="204"/>
+      <c r="J11" s="205"/>
       <c r="K11"/>
       <c r="L11"/>
       <c r="M11"/>
@@ -7826,14 +7826,14 @@
       <c r="B12" s="142" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="224"/>
-      <c r="D12" s="225"/>
-      <c r="E12" s="224"/>
-      <c r="F12" s="225"/>
-      <c r="G12" s="224"/>
-      <c r="H12" s="225"/>
-      <c r="I12" s="224"/>
-      <c r="J12" s="225"/>
+      <c r="C12" s="202"/>
+      <c r="D12" s="203"/>
+      <c r="E12" s="202"/>
+      <c r="F12" s="203"/>
+      <c r="G12" s="202"/>
+      <c r="H12" s="203"/>
+      <c r="I12" s="202"/>
+      <c r="J12" s="203"/>
       <c r="K12"/>
       <c r="L12"/>
       <c r="M12"/>
@@ -7844,14 +7844,14 @@
       <c r="B13" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="222"/>
-      <c r="D13" s="223"/>
-      <c r="E13" s="222"/>
-      <c r="F13" s="223"/>
-      <c r="G13" s="222"/>
-      <c r="H13" s="223"/>
-      <c r="I13" s="222"/>
-      <c r="J13" s="223"/>
+      <c r="C13" s="200"/>
+      <c r="D13" s="201"/>
+      <c r="E13" s="200"/>
+      <c r="F13" s="201"/>
+      <c r="G13" s="200"/>
+      <c r="H13" s="201"/>
+      <c r="I13" s="200"/>
+      <c r="J13" s="201"/>
       <c r="K13"/>
       <c r="L13"/>
       <c r="M13"/>
@@ -7862,14 +7862,14 @@
       <c r="B14" s="144" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="222"/>
-      <c r="D14" s="223"/>
-      <c r="E14" s="222"/>
-      <c r="F14" s="223"/>
-      <c r="G14" s="222"/>
-      <c r="H14" s="223"/>
-      <c r="I14" s="222"/>
-      <c r="J14" s="223"/>
+      <c r="C14" s="200"/>
+      <c r="D14" s="201"/>
+      <c r="E14" s="200"/>
+      <c r="F14" s="201"/>
+      <c r="G14" s="200"/>
+      <c r="H14" s="201"/>
+      <c r="I14" s="200"/>
+      <c r="J14" s="201"/>
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14"/>
@@ -7880,14 +7880,14 @@
       <c r="B15" s="142" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="222"/>
-      <c r="D15" s="223"/>
-      <c r="E15" s="222"/>
-      <c r="F15" s="223"/>
-      <c r="G15" s="222"/>
-      <c r="H15" s="223"/>
-      <c r="I15" s="222"/>
-      <c r="J15" s="223"/>
+      <c r="C15" s="200"/>
+      <c r="D15" s="201"/>
+      <c r="E15" s="200"/>
+      <c r="F15" s="201"/>
+      <c r="G15" s="200"/>
+      <c r="H15" s="201"/>
+      <c r="I15" s="200"/>
+      <c r="J15" s="201"/>
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15"/>
@@ -7898,14 +7898,14 @@
       <c r="B16" s="142" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="227"/>
-      <c r="D16" s="228"/>
-      <c r="E16" s="227"/>
-      <c r="F16" s="228"/>
-      <c r="G16" s="227"/>
-      <c r="H16" s="228"/>
-      <c r="I16" s="227"/>
-      <c r="J16" s="228"/>
+      <c r="C16" s="204"/>
+      <c r="D16" s="205"/>
+      <c r="E16" s="204"/>
+      <c r="F16" s="205"/>
+      <c r="G16" s="204"/>
+      <c r="H16" s="205"/>
+      <c r="I16" s="204"/>
+      <c r="J16" s="205"/>
       <c r="K16"/>
       <c r="L16"/>
       <c r="M16"/>
@@ -7916,14 +7916,14 @@
       <c r="B17" s="143" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="224"/>
-      <c r="D17" s="225"/>
-      <c r="E17" s="224"/>
-      <c r="F17" s="225"/>
-      <c r="G17" s="224"/>
-      <c r="H17" s="225"/>
-      <c r="I17" s="224"/>
-      <c r="J17" s="225"/>
+      <c r="C17" s="202"/>
+      <c r="D17" s="203"/>
+      <c r="E17" s="202"/>
+      <c r="F17" s="203"/>
+      <c r="G17" s="202"/>
+      <c r="H17" s="203"/>
+      <c r="I17" s="202"/>
+      <c r="J17" s="203"/>
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
@@ -7934,14 +7934,14 @@
       <c r="B18" s="144" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="222"/>
-      <c r="D18" s="223"/>
-      <c r="E18" s="222"/>
-      <c r="F18" s="223"/>
-      <c r="G18" s="222"/>
-      <c r="H18" s="223"/>
-      <c r="I18" s="222"/>
-      <c r="J18" s="223"/>
+      <c r="C18" s="200"/>
+      <c r="D18" s="201"/>
+      <c r="E18" s="200"/>
+      <c r="F18" s="201"/>
+      <c r="G18" s="200"/>
+      <c r="H18" s="201"/>
+      <c r="I18" s="200"/>
+      <c r="J18" s="201"/>
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
@@ -7952,14 +7952,14 @@
       <c r="B19" s="142" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="222"/>
-      <c r="D19" s="223"/>
-      <c r="E19" s="222"/>
-      <c r="F19" s="223"/>
-      <c r="G19" s="222"/>
-      <c r="H19" s="223"/>
-      <c r="I19" s="222"/>
-      <c r="J19" s="223"/>
+      <c r="C19" s="200"/>
+      <c r="D19" s="201"/>
+      <c r="E19" s="200"/>
+      <c r="F19" s="201"/>
+      <c r="G19" s="200"/>
+      <c r="H19" s="201"/>
+      <c r="I19" s="200"/>
+      <c r="J19" s="201"/>
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19"/>
@@ -7967,17 +7967,17 @@
     </row>
     <row r="20" spans="1:14" s="27" customFormat="1" ht="15">
       <c r="A20" s="135"/>
-      <c r="B20" s="199" t="s">
+      <c r="B20" s="218" t="s">
         <v>455</v>
       </c>
-      <c r="C20" s="201"/>
-      <c r="D20" s="202"/>
-      <c r="E20" s="201"/>
-      <c r="F20" s="202"/>
-      <c r="G20" s="201"/>
-      <c r="H20" s="202"/>
-      <c r="I20" s="201"/>
-      <c r="J20" s="202"/>
+      <c r="C20" s="220"/>
+      <c r="D20" s="221"/>
+      <c r="E20" s="220"/>
+      <c r="F20" s="221"/>
+      <c r="G20" s="220"/>
+      <c r="H20" s="221"/>
+      <c r="I20" s="220"/>
+      <c r="J20" s="221"/>
       <c r="K20"/>
       <c r="L20"/>
       <c r="M20"/>
@@ -7985,15 +7985,15 @@
     </row>
     <row r="21" spans="1:14" s="27" customFormat="1" ht="16" thickBot="1">
       <c r="A21" s="135"/>
-      <c r="B21" s="200"/>
-      <c r="C21" s="203"/>
-      <c r="D21" s="204"/>
-      <c r="E21" s="203"/>
-      <c r="F21" s="204"/>
-      <c r="G21" s="203"/>
-      <c r="H21" s="204"/>
-      <c r="I21" s="203"/>
-      <c r="J21" s="204"/>
+      <c r="B21" s="219"/>
+      <c r="C21" s="222"/>
+      <c r="D21" s="223"/>
+      <c r="E21" s="222"/>
+      <c r="F21" s="223"/>
+      <c r="G21" s="222"/>
+      <c r="H21" s="223"/>
+      <c r="I21" s="222"/>
+      <c r="J21" s="223"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
@@ -8004,14 +8004,14 @@
       <c r="B22" s="198" t="s">
         <v>456</v>
       </c>
-      <c r="C22" s="205"/>
-      <c r="D22" s="206"/>
-      <c r="E22" s="205"/>
-      <c r="F22" s="206"/>
-      <c r="G22" s="205"/>
-      <c r="H22" s="206"/>
-      <c r="I22" s="205"/>
-      <c r="J22" s="206"/>
+      <c r="C22" s="224"/>
+      <c r="D22" s="225"/>
+      <c r="E22" s="224"/>
+      <c r="F22" s="225"/>
+      <c r="G22" s="224"/>
+      <c r="H22" s="225"/>
+      <c r="I22" s="224"/>
+      <c r="J22" s="225"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
@@ -8020,14 +8020,14 @@
     <row r="23" spans="1:14" s="27" customFormat="1" ht="15">
       <c r="A23" s="135"/>
       <c r="B23" s="133"/>
-      <c r="C23" s="207"/>
-      <c r="D23" s="208"/>
-      <c r="E23" s="207"/>
-      <c r="F23" s="208"/>
-      <c r="G23" s="207"/>
-      <c r="H23" s="208"/>
-      <c r="I23" s="207"/>
-      <c r="J23" s="208"/>
+      <c r="C23" s="226"/>
+      <c r="D23" s="227"/>
+      <c r="E23" s="226"/>
+      <c r="F23" s="227"/>
+      <c r="G23" s="226"/>
+      <c r="H23" s="227"/>
+      <c r="I23" s="226"/>
+      <c r="J23" s="227"/>
       <c r="K23"/>
       <c r="L23"/>
       <c r="M23"/>
@@ -8036,14 +8036,14 @@
     <row r="24" spans="1:14" s="27" customFormat="1" ht="15">
       <c r="A24" s="135"/>
       <c r="B24" s="133"/>
-      <c r="C24" s="207"/>
-      <c r="D24" s="208"/>
-      <c r="E24" s="207"/>
-      <c r="F24" s="208"/>
-      <c r="G24" s="207"/>
-      <c r="H24" s="208"/>
-      <c r="I24" s="207"/>
-      <c r="J24" s="208"/>
+      <c r="C24" s="226"/>
+      <c r="D24" s="227"/>
+      <c r="E24" s="226"/>
+      <c r="F24" s="227"/>
+      <c r="G24" s="226"/>
+      <c r="H24" s="227"/>
+      <c r="I24" s="226"/>
+      <c r="J24" s="227"/>
       <c r="K24"/>
       <c r="L24"/>
       <c r="M24"/>
@@ -8052,14 +8052,14 @@
     <row r="25" spans="1:14" s="27" customFormat="1" ht="15">
       <c r="A25" s="135"/>
       <c r="B25" s="133"/>
-      <c r="C25" s="207"/>
-      <c r="D25" s="208"/>
-      <c r="E25" s="207"/>
-      <c r="F25" s="208"/>
-      <c r="G25" s="207"/>
-      <c r="H25" s="208"/>
-      <c r="I25" s="207"/>
-      <c r="J25" s="208"/>
+      <c r="C25" s="226"/>
+      <c r="D25" s="227"/>
+      <c r="E25" s="226"/>
+      <c r="F25" s="227"/>
+      <c r="G25" s="226"/>
+      <c r="H25" s="227"/>
+      <c r="I25" s="226"/>
+      <c r="J25" s="227"/>
       <c r="K25"/>
       <c r="L25"/>
       <c r="M25"/>
@@ -8068,14 +8068,14 @@
     <row r="26" spans="1:14" s="27" customFormat="1" ht="16" thickBot="1">
       <c r="A26" s="135"/>
       <c r="B26" s="137"/>
-      <c r="C26" s="207"/>
-      <c r="D26" s="208"/>
-      <c r="E26" s="207"/>
-      <c r="F26" s="208"/>
-      <c r="G26" s="207"/>
-      <c r="H26" s="208"/>
-      <c r="I26" s="207"/>
-      <c r="J26" s="208"/>
+      <c r="C26" s="226"/>
+      <c r="D26" s="227"/>
+      <c r="E26" s="226"/>
+      <c r="F26" s="227"/>
+      <c r="G26" s="226"/>
+      <c r="H26" s="227"/>
+      <c r="I26" s="226"/>
+      <c r="J26" s="227"/>
       <c r="K26"/>
       <c r="L26"/>
       <c r="M26"/>
@@ -8084,14 +8084,14 @@
     <row r="27" spans="1:14" s="27" customFormat="1" ht="15">
       <c r="A27" s="135"/>
       <c r="B27" s="134"/>
-      <c r="C27" s="207"/>
-      <c r="D27" s="208"/>
-      <c r="E27" s="207"/>
-      <c r="F27" s="208"/>
-      <c r="G27" s="207"/>
-      <c r="H27" s="208"/>
-      <c r="I27" s="207"/>
-      <c r="J27" s="208"/>
+      <c r="C27" s="226"/>
+      <c r="D27" s="227"/>
+      <c r="E27" s="226"/>
+      <c r="F27" s="227"/>
+      <c r="G27" s="226"/>
+      <c r="H27" s="227"/>
+      <c r="I27" s="226"/>
+      <c r="J27" s="227"/>
       <c r="K27"/>
       <c r="L27"/>
       <c r="M27"/>
@@ -8100,14 +8100,14 @@
     <row r="28" spans="1:14" s="27" customFormat="1" ht="15">
       <c r="A28" s="135"/>
       <c r="B28" s="133"/>
-      <c r="C28" s="207"/>
-      <c r="D28" s="208"/>
-      <c r="E28" s="207"/>
-      <c r="F28" s="208"/>
-      <c r="G28" s="207"/>
-      <c r="H28" s="208"/>
-      <c r="I28" s="207"/>
-      <c r="J28" s="208"/>
+      <c r="C28" s="226"/>
+      <c r="D28" s="227"/>
+      <c r="E28" s="226"/>
+      <c r="F28" s="227"/>
+      <c r="G28" s="226"/>
+      <c r="H28" s="227"/>
+      <c r="I28" s="226"/>
+      <c r="J28" s="227"/>
       <c r="K28"/>
       <c r="L28"/>
       <c r="M28"/>
@@ -8116,14 +8116,14 @@
     <row r="29" spans="1:14" s="27" customFormat="1" ht="15">
       <c r="A29" s="135"/>
       <c r="B29" s="133"/>
-      <c r="C29" s="207"/>
-      <c r="D29" s="208"/>
-      <c r="E29" s="207"/>
-      <c r="F29" s="208"/>
-      <c r="G29" s="207"/>
-      <c r="H29" s="208"/>
-      <c r="I29" s="207"/>
-      <c r="J29" s="208"/>
+      <c r="C29" s="226"/>
+      <c r="D29" s="227"/>
+      <c r="E29" s="226"/>
+      <c r="F29" s="227"/>
+      <c r="G29" s="226"/>
+      <c r="H29" s="227"/>
+      <c r="I29" s="226"/>
+      <c r="J29" s="227"/>
       <c r="K29"/>
       <c r="L29"/>
       <c r="M29"/>
@@ -8132,14 +8132,14 @@
     <row r="30" spans="1:14" s="27" customFormat="1" ht="15">
       <c r="A30" s="135"/>
       <c r="B30" s="133"/>
-      <c r="C30" s="207"/>
-      <c r="D30" s="208"/>
-      <c r="E30" s="207"/>
-      <c r="F30" s="208"/>
-      <c r="G30" s="207"/>
-      <c r="H30" s="208"/>
-      <c r="I30" s="207"/>
-      <c r="J30" s="208"/>
+      <c r="C30" s="226"/>
+      <c r="D30" s="227"/>
+      <c r="E30" s="226"/>
+      <c r="F30" s="227"/>
+      <c r="G30" s="226"/>
+      <c r="H30" s="227"/>
+      <c r="I30" s="226"/>
+      <c r="J30" s="227"/>
       <c r="K30"/>
       <c r="L30"/>
       <c r="M30"/>
@@ -8148,14 +8148,14 @@
     <row r="31" spans="1:14" s="27" customFormat="1" ht="16" thickBot="1">
       <c r="A31" s="135"/>
       <c r="B31" s="137"/>
-      <c r="C31" s="207"/>
-      <c r="D31" s="208"/>
-      <c r="E31" s="207"/>
-      <c r="F31" s="208"/>
-      <c r="G31" s="207"/>
-      <c r="H31" s="208"/>
-      <c r="I31" s="207"/>
-      <c r="J31" s="208"/>
+      <c r="C31" s="226"/>
+      <c r="D31" s="227"/>
+      <c r="E31" s="226"/>
+      <c r="F31" s="227"/>
+      <c r="G31" s="226"/>
+      <c r="H31" s="227"/>
+      <c r="I31" s="226"/>
+      <c r="J31" s="227"/>
       <c r="K31"/>
       <c r="L31"/>
       <c r="M31"/>
@@ -8164,14 +8164,14 @@
     <row r="32" spans="1:14" s="27" customFormat="1" ht="15">
       <c r="A32" s="135"/>
       <c r="B32" s="134"/>
-      <c r="C32" s="207"/>
-      <c r="D32" s="208"/>
-      <c r="E32" s="207"/>
-      <c r="F32" s="208"/>
-      <c r="G32" s="207"/>
-      <c r="H32" s="208"/>
-      <c r="I32" s="207"/>
-      <c r="J32" s="208"/>
+      <c r="C32" s="226"/>
+      <c r="D32" s="227"/>
+      <c r="E32" s="226"/>
+      <c r="F32" s="227"/>
+      <c r="G32" s="226"/>
+      <c r="H32" s="227"/>
+      <c r="I32" s="226"/>
+      <c r="J32" s="227"/>
       <c r="K32"/>
       <c r="L32"/>
       <c r="M32"/>
@@ -8180,14 +8180,14 @@
     <row r="33" spans="1:18" s="27" customFormat="1" ht="15">
       <c r="A33" s="135"/>
       <c r="B33" s="133"/>
-      <c r="C33" s="207"/>
-      <c r="D33" s="208"/>
-      <c r="E33" s="207"/>
-      <c r="F33" s="208"/>
-      <c r="G33" s="207"/>
-      <c r="H33" s="208"/>
-      <c r="I33" s="207"/>
-      <c r="J33" s="208"/>
+      <c r="C33" s="226"/>
+      <c r="D33" s="227"/>
+      <c r="E33" s="226"/>
+      <c r="F33" s="227"/>
+      <c r="G33" s="226"/>
+      <c r="H33" s="227"/>
+      <c r="I33" s="226"/>
+      <c r="J33" s="227"/>
       <c r="K33"/>
       <c r="L33"/>
       <c r="M33"/>
@@ -8196,14 +8196,14 @@
     <row r="34" spans="1:18" s="27" customFormat="1" ht="15">
       <c r="A34" s="135"/>
       <c r="B34" s="133"/>
-      <c r="C34" s="207"/>
-      <c r="D34" s="208"/>
-      <c r="E34" s="207"/>
-      <c r="F34" s="208"/>
-      <c r="G34" s="207"/>
-      <c r="H34" s="208"/>
-      <c r="I34" s="207"/>
-      <c r="J34" s="208"/>
+      <c r="C34" s="226"/>
+      <c r="D34" s="227"/>
+      <c r="E34" s="226"/>
+      <c r="F34" s="227"/>
+      <c r="G34" s="226"/>
+      <c r="H34" s="227"/>
+      <c r="I34" s="226"/>
+      <c r="J34" s="227"/>
       <c r="K34"/>
       <c r="L34"/>
       <c r="M34"/>
@@ -8212,14 +8212,14 @@
     <row r="35" spans="1:18" s="27" customFormat="1" ht="15">
       <c r="A35" s="135"/>
       <c r="B35" s="133"/>
-      <c r="C35" s="207"/>
-      <c r="D35" s="208"/>
-      <c r="E35" s="207"/>
-      <c r="F35" s="208"/>
-      <c r="G35" s="207"/>
-      <c r="H35" s="208"/>
-      <c r="I35" s="207"/>
-      <c r="J35" s="208"/>
+      <c r="C35" s="226"/>
+      <c r="D35" s="227"/>
+      <c r="E35" s="226"/>
+      <c r="F35" s="227"/>
+      <c r="G35" s="226"/>
+      <c r="H35" s="227"/>
+      <c r="I35" s="226"/>
+      <c r="J35" s="227"/>
       <c r="K35"/>
       <c r="L35"/>
       <c r="M35"/>
@@ -8228,14 +8228,14 @@
     <row r="36" spans="1:18" s="27" customFormat="1" ht="16" thickBot="1">
       <c r="A36" s="135"/>
       <c r="B36" s="137"/>
-      <c r="C36" s="207"/>
-      <c r="D36" s="208"/>
-      <c r="E36" s="207"/>
-      <c r="F36" s="208"/>
-      <c r="G36" s="207"/>
-      <c r="H36" s="208"/>
-      <c r="I36" s="207"/>
-      <c r="J36" s="208"/>
+      <c r="C36" s="226"/>
+      <c r="D36" s="227"/>
+      <c r="E36" s="226"/>
+      <c r="F36" s="227"/>
+      <c r="G36" s="226"/>
+      <c r="H36" s="227"/>
+      <c r="I36" s="226"/>
+      <c r="J36" s="227"/>
       <c r="K36"/>
       <c r="L36"/>
       <c r="M36"/>
@@ -8244,14 +8244,14 @@
     <row r="37" spans="1:18" s="27" customFormat="1" ht="15">
       <c r="A37" s="135"/>
       <c r="B37" s="134"/>
-      <c r="C37" s="207"/>
-      <c r="D37" s="208"/>
-      <c r="E37" s="207"/>
-      <c r="F37" s="208"/>
-      <c r="G37" s="207"/>
-      <c r="H37" s="208"/>
-      <c r="I37" s="207"/>
-      <c r="J37" s="208"/>
+      <c r="C37" s="226"/>
+      <c r="D37" s="227"/>
+      <c r="E37" s="226"/>
+      <c r="F37" s="227"/>
+      <c r="G37" s="226"/>
+      <c r="H37" s="227"/>
+      <c r="I37" s="226"/>
+      <c r="J37" s="227"/>
       <c r="K37"/>
       <c r="L37"/>
       <c r="M37"/>
@@ -8260,14 +8260,14 @@
     <row r="38" spans="1:18" s="27" customFormat="1" ht="15">
       <c r="A38" s="135"/>
       <c r="B38" s="133"/>
-      <c r="C38" s="207"/>
-      <c r="D38" s="208"/>
-      <c r="E38" s="207"/>
-      <c r="F38" s="208"/>
-      <c r="G38" s="207"/>
-      <c r="H38" s="208"/>
-      <c r="I38" s="207"/>
-      <c r="J38" s="208"/>
+      <c r="C38" s="226"/>
+      <c r="D38" s="227"/>
+      <c r="E38" s="226"/>
+      <c r="F38" s="227"/>
+      <c r="G38" s="226"/>
+      <c r="H38" s="227"/>
+      <c r="I38" s="226"/>
+      <c r="J38" s="227"/>
       <c r="K38"/>
       <c r="L38"/>
       <c r="M38"/>
@@ -8276,14 +8276,14 @@
     <row r="39" spans="1:18" s="27" customFormat="1" ht="15">
       <c r="A39" s="135"/>
       <c r="B39" s="133"/>
-      <c r="C39" s="207"/>
-      <c r="D39" s="208"/>
-      <c r="E39" s="207"/>
-      <c r="F39" s="208"/>
-      <c r="G39" s="207"/>
-      <c r="H39" s="208"/>
-      <c r="I39" s="207"/>
-      <c r="J39" s="208"/>
+      <c r="C39" s="226"/>
+      <c r="D39" s="227"/>
+      <c r="E39" s="226"/>
+      <c r="F39" s="227"/>
+      <c r="G39" s="226"/>
+      <c r="H39" s="227"/>
+      <c r="I39" s="226"/>
+      <c r="J39" s="227"/>
       <c r="K39"/>
       <c r="L39"/>
       <c r="M39"/>
@@ -8292,14 +8292,14 @@
     <row r="40" spans="1:18" s="27" customFormat="1" ht="15">
       <c r="A40" s="135"/>
       <c r="B40" s="133"/>
-      <c r="C40" s="207"/>
-      <c r="D40" s="208"/>
-      <c r="E40" s="207"/>
-      <c r="F40" s="208"/>
-      <c r="G40" s="207"/>
-      <c r="H40" s="208"/>
-      <c r="I40" s="207"/>
-      <c r="J40" s="208"/>
+      <c r="C40" s="226"/>
+      <c r="D40" s="227"/>
+      <c r="E40" s="226"/>
+      <c r="F40" s="227"/>
+      <c r="G40" s="226"/>
+      <c r="H40" s="227"/>
+      <c r="I40" s="226"/>
+      <c r="J40" s="227"/>
       <c r="K40"/>
       <c r="L40"/>
       <c r="M40"/>
@@ -8308,14 +8308,14 @@
     <row r="41" spans="1:18" s="27" customFormat="1" ht="16" thickBot="1">
       <c r="A41" s="135"/>
       <c r="B41" s="137"/>
-      <c r="C41" s="209"/>
-      <c r="D41" s="210"/>
-      <c r="E41" s="209"/>
-      <c r="F41" s="210"/>
-      <c r="G41" s="209"/>
-      <c r="H41" s="210"/>
-      <c r="I41" s="209"/>
-      <c r="J41" s="210"/>
+      <c r="C41" s="228"/>
+      <c r="D41" s="229"/>
+      <c r="E41" s="228"/>
+      <c r="F41" s="229"/>
+      <c r="G41" s="228"/>
+      <c r="H41" s="229"/>
+      <c r="I41" s="228"/>
+      <c r="J41" s="229"/>
       <c r="K41"/>
       <c r="L41"/>
       <c r="M41"/>
@@ -8809,38 +8809,30 @@
     <row r="86" ht="9.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C22:D41"/>
+    <mergeCell ref="E22:F41"/>
+    <mergeCell ref="G22:H41"/>
+    <mergeCell ref="I22:J41"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E20:F21"/>
+    <mergeCell ref="G20:H21"/>
+    <mergeCell ref="I20:J21"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="H1:I2"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:H11"/>
@@ -8857,30 +8849,38 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="H1:I2"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="E20:F21"/>
-    <mergeCell ref="G20:H21"/>
-    <mergeCell ref="I20:J21"/>
-    <mergeCell ref="C22:D41"/>
-    <mergeCell ref="E22:F41"/>
-    <mergeCell ref="G22:H41"/>
-    <mergeCell ref="I22:J41"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
   </mergeCells>
   <phoneticPr fontId="33" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -8905,7 +8905,7 @@
   </sheetPr>
   <dimension ref="A1:R86"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -8918,47 +8918,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="29" customFormat="1" ht="12" customHeight="1">
-      <c r="B1" s="213" t="s">
+      <c r="B1" s="209" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="213"/>
-      <c r="D1" s="234" t="s">
+      <c r="C1" s="209"/>
+      <c r="D1" s="235" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="235" t="s">
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="236" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="235"/>
-      <c r="I1" s="235"/>
-      <c r="J1" s="213" t="s">
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="209" t="s">
         <v>247</v>
       </c>
-      <c r="K1" s="213"/>
-      <c r="L1" s="213"/>
-      <c r="M1" s="232" t="s">
+      <c r="K1" s="209"/>
+      <c r="L1" s="209"/>
+      <c r="M1" s="233" t="s">
         <v>248</v>
       </c>
-      <c r="N1" s="233"/>
+      <c r="N1" s="234"/>
       <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" s="29" customFormat="1" ht="12" customHeight="1">
-      <c r="B2" s="213"/>
-      <c r="C2" s="213"/>
-      <c r="D2" s="234"/>
-      <c r="E2" s="234"/>
-      <c r="F2" s="234"/>
-      <c r="G2" s="235"/>
-      <c r="H2" s="235"/>
-      <c r="I2" s="235"/>
-      <c r="J2" s="213"/>
-      <c r="K2" s="213"/>
-      <c r="L2" s="213"/>
-      <c r="M2" s="232" t="s">
+      <c r="B2" s="209"/>
+      <c r="C2" s="209"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="235"/>
+      <c r="F2" s="235"/>
+      <c r="G2" s="236"/>
+      <c r="H2" s="236"/>
+      <c r="I2" s="236"/>
+      <c r="J2" s="209"/>
+      <c r="K2" s="209"/>
+      <c r="L2" s="209"/>
+      <c r="M2" s="233" t="s">
         <v>246</v>
       </c>
-      <c r="N2" s="233"/>
+      <c r="N2" s="234"/>
       <c r="O2" s="44"/>
     </row>
     <row r="3" spans="1:15" s="63" customFormat="1" ht="16" customHeight="1">
@@ -8994,10 +8994,10 @@
       <c r="N4" s="67"/>
     </row>
     <row r="5" spans="1:15" s="27" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="229" t="s">
+      <c r="A5" s="230" t="s">
         <v>160</v>
       </c>
-      <c r="B5" s="230"/>
+      <c r="B5" s="231"/>
       <c r="C5" s="8" t="s">
         <v>120</v>
       </c>
@@ -10363,10 +10363,10 @@
       <c r="H67" s="28"/>
       <c r="I67" s="28"/>
       <c r="J67" s="65"/>
-      <c r="K67" s="231" t="s">
+      <c r="K67" s="232" t="s">
         <v>13</v>
       </c>
-      <c r="L67" s="231"/>
+      <c r="L67" s="232"/>
       <c r="M67" s="28"/>
       <c r="N67" s="35"/>
     </row>
@@ -10466,7 +10466,7 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A21" zoomScale="150" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="150" workbookViewId="0">
       <selection activeCell="A39" sqref="A39:A40"/>
     </sheetView>
   </sheetViews>
@@ -10477,46 +10477,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="209" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="213"/>
-      <c r="C1" s="234" t="s">
+      <c r="B1" s="209"/>
+      <c r="C1" s="235" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
-      <c r="F1" s="235" t="s">
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="236" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="235"/>
-      <c r="H1" s="235"/>
-      <c r="I1" s="213" t="s">
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="209" t="s">
         <v>247</v>
       </c>
-      <c r="J1" s="213"/>
-      <c r="K1" s="213"/>
-      <c r="L1" s="232" t="s">
+      <c r="J1" s="209"/>
+      <c r="K1" s="209"/>
+      <c r="L1" s="233" t="s">
         <v>248</v>
       </c>
-      <c r="M1" s="233"/>
+      <c r="M1" s="234"/>
     </row>
     <row r="2" spans="1:13" ht="13">
-      <c r="A2" s="213"/>
-      <c r="B2" s="213"/>
-      <c r="C2" s="234"/>
-      <c r="D2" s="234"/>
-      <c r="E2" s="234"/>
-      <c r="F2" s="235"/>
-      <c r="G2" s="235"/>
-      <c r="H2" s="235"/>
-      <c r="I2" s="213"/>
-      <c r="J2" s="213"/>
-      <c r="K2" s="213"/>
-      <c r="L2" s="232" t="s">
+      <c r="A2" s="209"/>
+      <c r="B2" s="209"/>
+      <c r="C2" s="235"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="235"/>
+      <c r="F2" s="236"/>
+      <c r="G2" s="236"/>
+      <c r="H2" s="236"/>
+      <c r="I2" s="209"/>
+      <c r="J2" s="209"/>
+      <c r="K2" s="209"/>
+      <c r="L2" s="233" t="s">
         <v>246</v>
       </c>
-      <c r="M2" s="233"/>
+      <c r="M2" s="234"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="72" t="s">
@@ -11267,7 +11267,7 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="88" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="89" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;LKEEN of New England_x000D_KEEN Lab PI_x000D_Southern GOM&amp;C&amp;"Arial Narrow,Bold"&amp;12KEEN Kelp Removal Experiment_x000D_UPC Data Sheet</oddHeader>
     <oddFooter>&amp;L&amp;F&amp;RUpdated &amp;D</oddFooter>
@@ -11287,7 +11287,7 @@
   </sheetPr>
   <dimension ref="A1:CX107"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A36" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A36" zoomScale="150" workbookViewId="0">
       <selection activeCell="BP55" sqref="BP55"/>
     </sheetView>
   </sheetViews>
@@ -16815,7 +16815,7 @@
   </sheetData>
   <phoneticPr fontId="33" type="noConversion"/>
   <pageMargins left="0.56999999999999995" right="0.5" top="0.52" bottom="0.52" header="0.15" footer="0.15"/>
-  <pageSetup scale="81" orientation="portrait"/>
+  <pageSetup scale="80" orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;8KEEN Gulf of Maine &amp; E. Canada_x000D_KEEN Lab PI&amp;C&amp;"Arial,Bold"&amp;12 Sample UNIFORM POINT CONTACT_x000D_SPECIES LIST_x000D_</oddHeader>
     <oddFooter>&amp;L&amp;8&amp;F&amp;R&amp;8Updated &amp;D</oddFooter>

</xml_diff>